<commit_message>
added SA experiments results to excel file
</commit_message>
<xml_diff>
--- a/lab02/experiments/experiments.xlsx
+++ b/lab02/experiments/experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\SEM5\MHE\lab02\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\MHE\lab02\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7D3D20-2C29-41D5-8E21-40AE8CE6163D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD09F7-CB58-49CE-A0AA-59ED701B49DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="15">
   <si>
     <t xml:space="preserve">Taboo search duration: </t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>brute</t>
+  </si>
+  <si>
+    <t>Avg: Goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated annealing duration: </t>
+  </si>
+  <si>
+    <t>SA</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -607,6 +616,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -652,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,6 +782,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1123,6 +1181,64 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>SA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>taboo_M!$J$21:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.0692800000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3260799999999978E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2563119999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2688720000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-46C0-4CF3-97AC-00E82A97D307}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1336,7 +1452,653 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Average goal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> value f</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>or</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> 6, 9, 12, 24 numbers</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15014917125130992"/>
+          <c:y val="8.9045561673208914E-2"/>
+          <c:w val="0.84985082874869011"/>
+          <c:h val="0.79053154508024948"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Taboo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>taboo_M!$I$8:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>taboo_M!$J$38:$J$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0756-4FA0-BC77-8F930AB7BD10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hill climb</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>taboo_M!$I$8:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>taboo_M!$J$42:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.959999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0756-4FA0-BC77-8F930AB7BD10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Brute Force</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>taboo_M!$I$8:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>taboo_M!$J$47:$J$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0756-4FA0-BC77-8F930AB7BD10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>SA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>taboo_M!$J$51:$J$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0756-4FA0-BC77-8F930AB7BD10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1184486752"/>
+        <c:axId val="1184465536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1184486752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1184465536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1184465536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1184486752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1879,20 +2641,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85573</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5120</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3076423</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>71795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>411381</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>93876</xdr:rowOff>
+      <xdr:colOff>297081</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>160551</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1912,6 +3177,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>335333</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>79231</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2979D53E-D763-45CC-8A76-050CD40EA815}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2217,10 +3520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J290"/>
+  <dimension ref="A1:K398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O72" sqref="O72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2653,7 +3956,7 @@
         <v>1.2387200000000002E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2680,7 +3983,7 @@
         <v>3.5293639999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +4010,7 @@
         <v>0.193741424</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2727,7 +4030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2746,8 +4049,17 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="4">
+        <v>6</v>
+      </c>
+      <c r="J21" s="5">
+        <v>5.0692800000000002E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2766,8 +4078,15 @@
       <c r="F22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="18"/>
+      <c r="I22" s="8">
+        <v>9</v>
+      </c>
+      <c r="J22" s="9">
+        <v>6.3260799999999978E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2786,8 +4105,15 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="18"/>
+      <c r="I23" s="8">
+        <v>12</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1.2563119999999999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2806,8 +4132,18 @@
       <c r="F24">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="22"/>
+      <c r="I24" s="23">
+        <v>24</v>
+      </c>
+      <c r="J24" s="32">
+        <v>1.2688720000000001E-3</v>
+      </c>
+      <c r="K24" s="16">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2826,8 +4162,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
@@ -2844,11 +4183,17 @@
         <f>SUM(F1:F25)/25</f>
         <v>10.039999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2867,8 +4212,11 @@
       <c r="F28" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2887,8 +4235,11 @@
       <c r="F29" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2907,8 +4258,11 @@
       <c r="F30" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2927,8 +4281,11 @@
       <c r="F31" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2947,8 +4304,11 @@
       <c r="F32" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2967,8 +4327,11 @@
       <c r="F33" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2987,8 +4350,11 @@
       <c r="F34" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -3008,7 +4374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -3028,7 +4394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -3047,8 +4413,15 @@
       <c r="F37" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37" s="29"/>
+      <c r="I37" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -3067,8 +4440,17 @@
       <c r="F38" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="8">
+        <v>6</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -3087,8 +4469,15 @@
       <c r="F39" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" s="18"/>
+      <c r="I39" s="8">
+        <v>9</v>
+      </c>
+      <c r="J39" s="9">
+        <v>10.039999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -3107,8 +4496,15 @@
       <c r="F40" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40" s="18"/>
+      <c r="I40" s="8">
+        <v>12</v>
+      </c>
+      <c r="J40" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -3127,8 +4523,15 @@
       <c r="F41" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41" s="22"/>
+      <c r="I41" s="23">
+        <v>24</v>
+      </c>
+      <c r="J41" s="24">
+        <v>58.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -3147,8 +4550,17 @@
       <c r="F42" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="4">
+        <v>6</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -3167,8 +4579,15 @@
       <c r="F43" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43" s="18"/>
+      <c r="I43" s="8">
+        <v>9</v>
+      </c>
+      <c r="J43" s="9">
+        <v>8.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -3187,8 +4606,15 @@
       <c r="F44" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44" s="18"/>
+      <c r="I44" s="8">
+        <v>12</v>
+      </c>
+      <c r="J44" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -3207,8 +4633,15 @@
       <c r="F45" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45" s="22"/>
+      <c r="I45" s="23">
+        <v>24</v>
+      </c>
+      <c r="J45" s="24">
+        <v>68.959999999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -3228,7 +4661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -3247,8 +4680,17 @@
       <c r="F47" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="4">
+        <v>6</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -3267,8 +4709,15 @@
       <c r="F48" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48" s="18"/>
+      <c r="I48" s="8">
+        <v>9</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -3287,8 +4736,15 @@
       <c r="F49" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49" s="22"/>
+      <c r="I49" s="23">
+        <v>12</v>
+      </c>
+      <c r="J49" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -3308,7 +4764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -3327,8 +4783,17 @@
       <c r="F51" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H51" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="4">
+        <v>6</v>
+      </c>
+      <c r="J51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -3347,8 +4812,15 @@
       <c r="F52" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H52" s="18"/>
+      <c r="I52" s="8">
+        <v>9</v>
+      </c>
+      <c r="J52" s="9">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>5</v>
       </c>
@@ -3365,8 +4837,15 @@
         <f>SUM(F28:F52)/25</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H53" s="18"/>
+      <c r="I53" s="8">
+        <v>12</v>
+      </c>
+      <c r="J53" s="9">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3385,8 +4864,15 @@
       <c r="F54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H54" s="22"/>
+      <c r="I54" s="23">
+        <v>24</v>
+      </c>
+      <c r="J54" s="24">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3406,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -3426,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +4932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -3466,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -3486,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -3506,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -3526,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -3546,7 +5032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -3566,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -7998,6 +9484,2078 @@
       <c r="F290" s="16">
         <f>SUM(F265:F289)/25</f>
         <v>58.16</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>13</v>
+      </c>
+      <c r="B292">
+        <v>4.8480000000000002E-4</v>
+      </c>
+      <c r="C292" t="s">
+        <v>1</v>
+      </c>
+      <c r="D292">
+        <v>6</v>
+      </c>
+      <c r="E292" t="s">
+        <v>2</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>13</v>
+      </c>
+      <c r="B293">
+        <v>5.2380000000000005E-4</v>
+      </c>
+      <c r="C293" t="s">
+        <v>1</v>
+      </c>
+      <c r="D293">
+        <v>6</v>
+      </c>
+      <c r="E293" t="s">
+        <v>2</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>13</v>
+      </c>
+      <c r="B294">
+        <v>8.2649999999999998E-4</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1</v>
+      </c>
+      <c r="D294">
+        <v>6</v>
+      </c>
+      <c r="E294" t="s">
+        <v>2</v>
+      </c>
+      <c r="F294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>13</v>
+      </c>
+      <c r="B295">
+        <v>8.1780000000000004E-4</v>
+      </c>
+      <c r="C295" t="s">
+        <v>1</v>
+      </c>
+      <c r="D295">
+        <v>6</v>
+      </c>
+      <c r="E295" t="s">
+        <v>2</v>
+      </c>
+      <c r="F295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>13</v>
+      </c>
+      <c r="B296">
+        <v>7.4989999999999996E-4</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1</v>
+      </c>
+      <c r="D296">
+        <v>6</v>
+      </c>
+      <c r="E296" t="s">
+        <v>2</v>
+      </c>
+      <c r="F296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>13</v>
+      </c>
+      <c r="B297">
+        <v>4.6349999999999999E-4</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1</v>
+      </c>
+      <c r="D297">
+        <v>6</v>
+      </c>
+      <c r="E297" t="s">
+        <v>2</v>
+      </c>
+      <c r="F297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>13</v>
+      </c>
+      <c r="B298">
+        <v>4.6069999999999998E-4</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1</v>
+      </c>
+      <c r="D298">
+        <v>6</v>
+      </c>
+      <c r="E298" t="s">
+        <v>2</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>13</v>
+      </c>
+      <c r="B299">
+        <v>4.661E-4</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1</v>
+      </c>
+      <c r="D299">
+        <v>6</v>
+      </c>
+      <c r="E299" t="s">
+        <v>2</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>13</v>
+      </c>
+      <c r="B300">
+        <v>4.6319999999999998E-4</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1</v>
+      </c>
+      <c r="D300">
+        <v>6</v>
+      </c>
+      <c r="E300" t="s">
+        <v>2</v>
+      </c>
+      <c r="F300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>13</v>
+      </c>
+      <c r="B301">
+        <v>4.6289999999999998E-4</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1</v>
+      </c>
+      <c r="D301">
+        <v>6</v>
+      </c>
+      <c r="E301" t="s">
+        <v>2</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>13</v>
+      </c>
+      <c r="B302">
+        <v>4.6509999999999998E-4</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1</v>
+      </c>
+      <c r="D302">
+        <v>6</v>
+      </c>
+      <c r="E302" t="s">
+        <v>2</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>13</v>
+      </c>
+      <c r="B303">
+        <v>4.64E-4</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1</v>
+      </c>
+      <c r="D303">
+        <v>6</v>
+      </c>
+      <c r="E303" t="s">
+        <v>2</v>
+      </c>
+      <c r="F303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>13</v>
+      </c>
+      <c r="B304">
+        <v>4.6420000000000001E-4</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1</v>
+      </c>
+      <c r="D304">
+        <v>6</v>
+      </c>
+      <c r="E304" t="s">
+        <v>2</v>
+      </c>
+      <c r="F304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>13</v>
+      </c>
+      <c r="B305">
+        <v>4.6319999999999998E-4</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1</v>
+      </c>
+      <c r="D305">
+        <v>6</v>
+      </c>
+      <c r="E305" t="s">
+        <v>2</v>
+      </c>
+      <c r="F305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>13</v>
+      </c>
+      <c r="B306">
+        <v>4.6069999999999998E-4</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1</v>
+      </c>
+      <c r="D306">
+        <v>6</v>
+      </c>
+      <c r="E306" t="s">
+        <v>2</v>
+      </c>
+      <c r="F306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>13</v>
+      </c>
+      <c r="B307">
+        <v>4.6430000000000001E-4</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1</v>
+      </c>
+      <c r="D307">
+        <v>6</v>
+      </c>
+      <c r="E307" t="s">
+        <v>2</v>
+      </c>
+      <c r="F307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>13</v>
+      </c>
+      <c r="B308">
+        <v>4.6109999999999999E-4</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1</v>
+      </c>
+      <c r="D308">
+        <v>6</v>
+      </c>
+      <c r="E308" t="s">
+        <v>2</v>
+      </c>
+      <c r="F308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>13</v>
+      </c>
+      <c r="B309">
+        <v>4.6129999999999999E-4</v>
+      </c>
+      <c r="C309" t="s">
+        <v>1</v>
+      </c>
+      <c r="D309">
+        <v>6</v>
+      </c>
+      <c r="E309" t="s">
+        <v>2</v>
+      </c>
+      <c r="F309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>13</v>
+      </c>
+      <c r="B310">
+        <v>4.6680000000000002E-4</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1</v>
+      </c>
+      <c r="D310">
+        <v>6</v>
+      </c>
+      <c r="E310" t="s">
+        <v>2</v>
+      </c>
+      <c r="F310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>13</v>
+      </c>
+      <c r="B311">
+        <v>4.6519999999999998E-4</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1</v>
+      </c>
+      <c r="D311">
+        <v>6</v>
+      </c>
+      <c r="E311" t="s">
+        <v>2</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>13</v>
+      </c>
+      <c r="B312">
+        <v>4.64E-4</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1</v>
+      </c>
+      <c r="D312">
+        <v>6</v>
+      </c>
+      <c r="E312" t="s">
+        <v>2</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>13</v>
+      </c>
+      <c r="B313">
+        <v>4.6139999999999999E-4</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1</v>
+      </c>
+      <c r="D313">
+        <v>6</v>
+      </c>
+      <c r="E313" t="s">
+        <v>2</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>13</v>
+      </c>
+      <c r="B314">
+        <v>4.6450000000000001E-4</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1</v>
+      </c>
+      <c r="D314">
+        <v>6</v>
+      </c>
+      <c r="E314" t="s">
+        <v>2</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>13</v>
+      </c>
+      <c r="B315">
+        <v>4.6309999999999998E-4</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1</v>
+      </c>
+      <c r="D315">
+        <v>6</v>
+      </c>
+      <c r="E315" t="s">
+        <v>2</v>
+      </c>
+      <c r="F315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>13</v>
+      </c>
+      <c r="B316">
+        <v>4.6509999999999998E-4</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1</v>
+      </c>
+      <c r="D316">
+        <v>6</v>
+      </c>
+      <c r="E316" t="s">
+        <v>2</v>
+      </c>
+      <c r="F316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B317" s="15">
+        <f>SUM(B292:B316)/25</f>
+        <v>5.0692800000000002E-4</v>
+      </c>
+      <c r="C317" s="11"/>
+      <c r="D317" s="11"/>
+      <c r="E317" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F317" s="16">
+        <f>SUM(F292:F316)/25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>13</v>
+      </c>
+      <c r="B319">
+        <v>7.0730000000000001E-4</v>
+      </c>
+      <c r="C319" t="s">
+        <v>1</v>
+      </c>
+      <c r="D319">
+        <v>9</v>
+      </c>
+      <c r="E319" t="s">
+        <v>2</v>
+      </c>
+      <c r="F319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>13</v>
+      </c>
+      <c r="B320">
+        <v>6.7650000000000002E-4</v>
+      </c>
+      <c r="C320" t="s">
+        <v>1</v>
+      </c>
+      <c r="D320">
+        <v>9</v>
+      </c>
+      <c r="E320" t="s">
+        <v>2</v>
+      </c>
+      <c r="F320">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>13</v>
+      </c>
+      <c r="B321">
+        <v>6.6089999999999996E-4</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1</v>
+      </c>
+      <c r="D321">
+        <v>9</v>
+      </c>
+      <c r="E321" t="s">
+        <v>2</v>
+      </c>
+      <c r="F321">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>13</v>
+      </c>
+      <c r="B322">
+        <v>6.1799999999999995E-4</v>
+      </c>
+      <c r="C322" t="s">
+        <v>1</v>
+      </c>
+      <c r="D322">
+        <v>9</v>
+      </c>
+      <c r="E322" t="s">
+        <v>2</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>13</v>
+      </c>
+      <c r="B323">
+        <v>6.2140000000000003E-4</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1</v>
+      </c>
+      <c r="D323">
+        <v>9</v>
+      </c>
+      <c r="E323" t="s">
+        <v>2</v>
+      </c>
+      <c r="F323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>13</v>
+      </c>
+      <c r="B324">
+        <v>6.2270000000000001E-4</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1</v>
+      </c>
+      <c r="D324">
+        <v>9</v>
+      </c>
+      <c r="E324" t="s">
+        <v>2</v>
+      </c>
+      <c r="F324">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>13</v>
+      </c>
+      <c r="B325">
+        <v>6.1589999999999995E-4</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1</v>
+      </c>
+      <c r="D325">
+        <v>9</v>
+      </c>
+      <c r="E325" t="s">
+        <v>2</v>
+      </c>
+      <c r="F325">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>13</v>
+      </c>
+      <c r="B326">
+        <v>6.1419999999999997E-4</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1</v>
+      </c>
+      <c r="D326">
+        <v>9</v>
+      </c>
+      <c r="E326" t="s">
+        <v>2</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>13</v>
+      </c>
+      <c r="B327">
+        <v>6.177E-4</v>
+      </c>
+      <c r="C327" t="s">
+        <v>1</v>
+      </c>
+      <c r="D327">
+        <v>9</v>
+      </c>
+      <c r="E327" t="s">
+        <v>2</v>
+      </c>
+      <c r="F327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>13</v>
+      </c>
+      <c r="B328">
+        <v>6.1689999999999998E-4</v>
+      </c>
+      <c r="C328" t="s">
+        <v>1</v>
+      </c>
+      <c r="D328">
+        <v>9</v>
+      </c>
+      <c r="E328" t="s">
+        <v>2</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>13</v>
+      </c>
+      <c r="B329">
+        <v>6.1169999999999996E-4</v>
+      </c>
+      <c r="C329" t="s">
+        <v>1</v>
+      </c>
+      <c r="D329">
+        <v>9</v>
+      </c>
+      <c r="E329" t="s">
+        <v>2</v>
+      </c>
+      <c r="F329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>13</v>
+      </c>
+      <c r="B330">
+        <v>6.6750000000000002E-4</v>
+      </c>
+      <c r="C330" t="s">
+        <v>1</v>
+      </c>
+      <c r="D330">
+        <v>9</v>
+      </c>
+      <c r="E330" t="s">
+        <v>2</v>
+      </c>
+      <c r="F330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>13</v>
+      </c>
+      <c r="B331">
+        <v>6.1919999999999998E-4</v>
+      </c>
+      <c r="C331" t="s">
+        <v>1</v>
+      </c>
+      <c r="D331">
+        <v>9</v>
+      </c>
+      <c r="E331" t="s">
+        <v>2</v>
+      </c>
+      <c r="F331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>13</v>
+      </c>
+      <c r="B332">
+        <v>6.2109999999999997E-4</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1</v>
+      </c>
+      <c r="D332">
+        <v>9</v>
+      </c>
+      <c r="E332" t="s">
+        <v>2</v>
+      </c>
+      <c r="F332">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>13</v>
+      </c>
+      <c r="B333">
+        <v>6.2109999999999997E-4</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1</v>
+      </c>
+      <c r="D333">
+        <v>9</v>
+      </c>
+      <c r="E333" t="s">
+        <v>2</v>
+      </c>
+      <c r="F333">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>13</v>
+      </c>
+      <c r="B334">
+        <v>6.8440000000000005E-4</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1</v>
+      </c>
+      <c r="D334">
+        <v>9</v>
+      </c>
+      <c r="E334" t="s">
+        <v>2</v>
+      </c>
+      <c r="F334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>13</v>
+      </c>
+      <c r="B335">
+        <v>6.1499999999999999E-4</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1</v>
+      </c>
+      <c r="D335">
+        <v>9</v>
+      </c>
+      <c r="E335" t="s">
+        <v>2</v>
+      </c>
+      <c r="F335">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>13</v>
+      </c>
+      <c r="B336">
+        <v>6.5709999999999998E-4</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1</v>
+      </c>
+      <c r="D336">
+        <v>9</v>
+      </c>
+      <c r="E336" t="s">
+        <v>2</v>
+      </c>
+      <c r="F336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>13</v>
+      </c>
+      <c r="B337">
+        <v>6.223E-4</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1</v>
+      </c>
+      <c r="D337">
+        <v>9</v>
+      </c>
+      <c r="E337" t="s">
+        <v>2</v>
+      </c>
+      <c r="F337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>13</v>
+      </c>
+      <c r="B338">
+        <v>6.1059999999999999E-4</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1</v>
+      </c>
+      <c r="D338">
+        <v>9</v>
+      </c>
+      <c r="E338" t="s">
+        <v>2</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>13</v>
+      </c>
+      <c r="B339">
+        <v>6.112E-4</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1</v>
+      </c>
+      <c r="D339">
+        <v>9</v>
+      </c>
+      <c r="E339" t="s">
+        <v>2</v>
+      </c>
+      <c r="F339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>13</v>
+      </c>
+      <c r="B340">
+        <v>6.1600000000000001E-4</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1</v>
+      </c>
+      <c r="D340">
+        <v>9</v>
+      </c>
+      <c r="E340" t="s">
+        <v>2</v>
+      </c>
+      <c r="F340">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>13</v>
+      </c>
+      <c r="B341">
+        <v>6.1600000000000001E-4</v>
+      </c>
+      <c r="C341" t="s">
+        <v>1</v>
+      </c>
+      <c r="D341">
+        <v>9</v>
+      </c>
+      <c r="E341" t="s">
+        <v>2</v>
+      </c>
+      <c r="F341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>13</v>
+      </c>
+      <c r="B342">
+        <v>6.1810000000000001E-4</v>
+      </c>
+      <c r="C342" t="s">
+        <v>1</v>
+      </c>
+      <c r="D342">
+        <v>9</v>
+      </c>
+      <c r="E342" t="s">
+        <v>2</v>
+      </c>
+      <c r="F342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>13</v>
+      </c>
+      <c r="B343">
+        <v>6.5240000000000003E-4</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1</v>
+      </c>
+      <c r="D343">
+        <v>9</v>
+      </c>
+      <c r="E343" t="s">
+        <v>2</v>
+      </c>
+      <c r="F343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A344" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B344" s="15">
+        <f>SUM(B319:B343)/25</f>
+        <v>6.3260799999999978E-4</v>
+      </c>
+      <c r="C344" s="11"/>
+      <c r="D344" s="11"/>
+      <c r="E344" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F344" s="16">
+        <f>SUM(F319:F343)/25</f>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>13</v>
+      </c>
+      <c r="B346">
+        <v>1.1969000000000001E-3</v>
+      </c>
+      <c r="C346" t="s">
+        <v>1</v>
+      </c>
+      <c r="D346">
+        <v>12</v>
+      </c>
+      <c r="E346" t="s">
+        <v>2</v>
+      </c>
+      <c r="F346">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>13</v>
+      </c>
+      <c r="B347">
+        <v>1.8201999999999999E-3</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1</v>
+      </c>
+      <c r="D347">
+        <v>12</v>
+      </c>
+      <c r="E347" t="s">
+        <v>2</v>
+      </c>
+      <c r="F347">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>13</v>
+      </c>
+      <c r="B348">
+        <v>1.4311E-3</v>
+      </c>
+      <c r="C348" t="s">
+        <v>1</v>
+      </c>
+      <c r="D348">
+        <v>12</v>
+      </c>
+      <c r="E348" t="s">
+        <v>2</v>
+      </c>
+      <c r="F348">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>13</v>
+      </c>
+      <c r="B349">
+        <v>1.0541000000000001E-3</v>
+      </c>
+      <c r="C349" t="s">
+        <v>1</v>
+      </c>
+      <c r="D349">
+        <v>12</v>
+      </c>
+      <c r="E349" t="s">
+        <v>2</v>
+      </c>
+      <c r="F349">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>13</v>
+      </c>
+      <c r="B350">
+        <v>5.2385000000000001E-3</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1</v>
+      </c>
+      <c r="D350">
+        <v>12</v>
+      </c>
+      <c r="E350" t="s">
+        <v>2</v>
+      </c>
+      <c r="F350">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>13</v>
+      </c>
+      <c r="B351">
+        <v>1.4051999999999999E-3</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1</v>
+      </c>
+      <c r="D351">
+        <v>12</v>
+      </c>
+      <c r="E351" t="s">
+        <v>2</v>
+      </c>
+      <c r="F351">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>13</v>
+      </c>
+      <c r="B352">
+        <v>9.9580000000000003E-4</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1</v>
+      </c>
+      <c r="D352">
+        <v>12</v>
+      </c>
+      <c r="E352" t="s">
+        <v>2</v>
+      </c>
+      <c r="F352">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>13</v>
+      </c>
+      <c r="B353">
+        <v>9.8989999999999994E-4</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1</v>
+      </c>
+      <c r="D353">
+        <v>12</v>
+      </c>
+      <c r="E353" t="s">
+        <v>2</v>
+      </c>
+      <c r="F353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>13</v>
+      </c>
+      <c r="B354">
+        <v>1.1054000000000001E-3</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1</v>
+      </c>
+      <c r="D354">
+        <v>12</v>
+      </c>
+      <c r="E354" t="s">
+        <v>2</v>
+      </c>
+      <c r="F354">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>13</v>
+      </c>
+      <c r="B355">
+        <v>1.1444999999999999E-3</v>
+      </c>
+      <c r="C355" t="s">
+        <v>1</v>
+      </c>
+      <c r="D355">
+        <v>12</v>
+      </c>
+      <c r="E355" t="s">
+        <v>2</v>
+      </c>
+      <c r="F355">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>13</v>
+      </c>
+      <c r="B356">
+        <v>1.0009999999999999E-3</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1</v>
+      </c>
+      <c r="D356">
+        <v>12</v>
+      </c>
+      <c r="E356" t="s">
+        <v>2</v>
+      </c>
+      <c r="F356">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>13</v>
+      </c>
+      <c r="B357">
+        <v>9.8539999999999999E-4</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1</v>
+      </c>
+      <c r="D357">
+        <v>12</v>
+      </c>
+      <c r="E357" t="s">
+        <v>2</v>
+      </c>
+      <c r="F357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>13</v>
+      </c>
+      <c r="B358">
+        <v>1.0005000000000001E-3</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1</v>
+      </c>
+      <c r="D358">
+        <v>12</v>
+      </c>
+      <c r="E358" t="s">
+        <v>2</v>
+      </c>
+      <c r="F358">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>13</v>
+      </c>
+      <c r="B359">
+        <v>1.0036000000000001E-3</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1</v>
+      </c>
+      <c r="D359">
+        <v>12</v>
+      </c>
+      <c r="E359" t="s">
+        <v>2</v>
+      </c>
+      <c r="F359">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>13</v>
+      </c>
+      <c r="B360">
+        <v>1.0028999999999999E-3</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1</v>
+      </c>
+      <c r="D360">
+        <v>12</v>
+      </c>
+      <c r="E360" t="s">
+        <v>2</v>
+      </c>
+      <c r="F360">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>13</v>
+      </c>
+      <c r="B361">
+        <v>1.0032000000000001E-3</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1</v>
+      </c>
+      <c r="D361">
+        <v>12</v>
+      </c>
+      <c r="E361" t="s">
+        <v>2</v>
+      </c>
+      <c r="F361">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>13</v>
+      </c>
+      <c r="B362">
+        <v>9.9620000000000004E-4</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1</v>
+      </c>
+      <c r="D362">
+        <v>12</v>
+      </c>
+      <c r="E362" t="s">
+        <v>2</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>13</v>
+      </c>
+      <c r="B363">
+        <v>9.9310000000000002E-4</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1</v>
+      </c>
+      <c r="D363">
+        <v>12</v>
+      </c>
+      <c r="E363" t="s">
+        <v>2</v>
+      </c>
+      <c r="F363">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>13</v>
+      </c>
+      <c r="B364">
+        <v>1.0051000000000001E-3</v>
+      </c>
+      <c r="C364" t="s">
+        <v>1</v>
+      </c>
+      <c r="D364">
+        <v>12</v>
+      </c>
+      <c r="E364" t="s">
+        <v>2</v>
+      </c>
+      <c r="F364">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>13</v>
+      </c>
+      <c r="B365">
+        <v>9.9770000000000002E-4</v>
+      </c>
+      <c r="C365" t="s">
+        <v>1</v>
+      </c>
+      <c r="D365">
+        <v>12</v>
+      </c>
+      <c r="E365" t="s">
+        <v>2</v>
+      </c>
+      <c r="F365">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>13</v>
+      </c>
+      <c r="B366">
+        <v>9.923E-4</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1</v>
+      </c>
+      <c r="D366">
+        <v>12</v>
+      </c>
+      <c r="E366" t="s">
+        <v>2</v>
+      </c>
+      <c r="F366">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>13</v>
+      </c>
+      <c r="B367">
+        <v>1.0272E-3</v>
+      </c>
+      <c r="C367" t="s">
+        <v>1</v>
+      </c>
+      <c r="D367">
+        <v>12</v>
+      </c>
+      <c r="E367" t="s">
+        <v>2</v>
+      </c>
+      <c r="F367">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>13</v>
+      </c>
+      <c r="B368">
+        <v>9.9329999999999991E-4</v>
+      </c>
+      <c r="C368" t="s">
+        <v>1</v>
+      </c>
+      <c r="D368">
+        <v>12</v>
+      </c>
+      <c r="E368" t="s">
+        <v>2</v>
+      </c>
+      <c r="F368">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>13</v>
+      </c>
+      <c r="B369">
+        <v>1.0196999999999999E-3</v>
+      </c>
+      <c r="C369" t="s">
+        <v>1</v>
+      </c>
+      <c r="D369">
+        <v>12</v>
+      </c>
+      <c r="E369" t="s">
+        <v>2</v>
+      </c>
+      <c r="F369">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>13</v>
+      </c>
+      <c r="B370">
+        <v>1.005E-3</v>
+      </c>
+      <c r="C370" t="s">
+        <v>1</v>
+      </c>
+      <c r="D370">
+        <v>12</v>
+      </c>
+      <c r="E370" t="s">
+        <v>2</v>
+      </c>
+      <c r="F370">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A371" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B371" s="15">
+        <f>SUM(B346:B370)/25</f>
+        <v>1.2563119999999999E-3</v>
+      </c>
+      <c r="C371" s="11"/>
+      <c r="D371" s="11"/>
+      <c r="E371" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F371" s="16">
+        <f>SUM(F346:F370)/25</f>
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>13</v>
+      </c>
+      <c r="B373">
+        <v>1.5265000000000001E-3</v>
+      </c>
+      <c r="C373" t="s">
+        <v>1</v>
+      </c>
+      <c r="D373">
+        <v>24</v>
+      </c>
+      <c r="E373" t="s">
+        <v>2</v>
+      </c>
+      <c r="F373">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>13</v>
+      </c>
+      <c r="B374">
+        <v>1.3859E-3</v>
+      </c>
+      <c r="C374" t="s">
+        <v>1</v>
+      </c>
+      <c r="D374">
+        <v>24</v>
+      </c>
+      <c r="E374" t="s">
+        <v>2</v>
+      </c>
+      <c r="F374">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>13</v>
+      </c>
+      <c r="B375">
+        <v>1.3542999999999999E-3</v>
+      </c>
+      <c r="C375" t="s">
+        <v>1</v>
+      </c>
+      <c r="D375">
+        <v>24</v>
+      </c>
+      <c r="E375" t="s">
+        <v>2</v>
+      </c>
+      <c r="F375">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>13</v>
+      </c>
+      <c r="B376">
+        <v>1.2741E-3</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1</v>
+      </c>
+      <c r="D376">
+        <v>24</v>
+      </c>
+      <c r="E376" t="s">
+        <v>2</v>
+      </c>
+      <c r="F376">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>13</v>
+      </c>
+      <c r="B377">
+        <v>1.2495E-3</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1</v>
+      </c>
+      <c r="D377">
+        <v>24</v>
+      </c>
+      <c r="E377" t="s">
+        <v>2</v>
+      </c>
+      <c r="F377">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>13</v>
+      </c>
+      <c r="B378">
+        <v>1.2317000000000001E-3</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1</v>
+      </c>
+      <c r="D378">
+        <v>24</v>
+      </c>
+      <c r="E378" t="s">
+        <v>2</v>
+      </c>
+      <c r="F378">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>13</v>
+      </c>
+      <c r="B379">
+        <v>1.2405999999999999E-3</v>
+      </c>
+      <c r="C379" t="s">
+        <v>1</v>
+      </c>
+      <c r="D379">
+        <v>24</v>
+      </c>
+      <c r="E379" t="s">
+        <v>2</v>
+      </c>
+      <c r="F379">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>13</v>
+      </c>
+      <c r="B380">
+        <v>1.2172000000000001E-3</v>
+      </c>
+      <c r="C380" t="s">
+        <v>1</v>
+      </c>
+      <c r="D380">
+        <v>24</v>
+      </c>
+      <c r="E380" t="s">
+        <v>2</v>
+      </c>
+      <c r="F380">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>13</v>
+      </c>
+      <c r="B381">
+        <v>1.2289E-3</v>
+      </c>
+      <c r="C381" t="s">
+        <v>1</v>
+      </c>
+      <c r="D381">
+        <v>24</v>
+      </c>
+      <c r="E381" t="s">
+        <v>2</v>
+      </c>
+      <c r="F381">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>13</v>
+      </c>
+      <c r="B382">
+        <v>1.2346E-3</v>
+      </c>
+      <c r="C382" t="s">
+        <v>1</v>
+      </c>
+      <c r="D382">
+        <v>24</v>
+      </c>
+      <c r="E382" t="s">
+        <v>2</v>
+      </c>
+      <c r="F382">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>13</v>
+      </c>
+      <c r="B383">
+        <v>1.2329000000000001E-3</v>
+      </c>
+      <c r="C383" t="s">
+        <v>1</v>
+      </c>
+      <c r="D383">
+        <v>24</v>
+      </c>
+      <c r="E383" t="s">
+        <v>2</v>
+      </c>
+      <c r="F383">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>13</v>
+      </c>
+      <c r="B384">
+        <v>1.2232E-3</v>
+      </c>
+      <c r="C384" t="s">
+        <v>1</v>
+      </c>
+      <c r="D384">
+        <v>24</v>
+      </c>
+      <c r="E384" t="s">
+        <v>2</v>
+      </c>
+      <c r="F384">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>13</v>
+      </c>
+      <c r="B385">
+        <v>1.2290000000000001E-3</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1</v>
+      </c>
+      <c r="D385">
+        <v>24</v>
+      </c>
+      <c r="E385" t="s">
+        <v>2</v>
+      </c>
+      <c r="F385">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>13</v>
+      </c>
+      <c r="B386">
+        <v>1.2363999999999999E-3</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1</v>
+      </c>
+      <c r="D386">
+        <v>24</v>
+      </c>
+      <c r="E386" t="s">
+        <v>2</v>
+      </c>
+      <c r="F386">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>13</v>
+      </c>
+      <c r="B387">
+        <v>1.2738999999999999E-3</v>
+      </c>
+      <c r="C387" t="s">
+        <v>1</v>
+      </c>
+      <c r="D387">
+        <v>24</v>
+      </c>
+      <c r="E387" t="s">
+        <v>2</v>
+      </c>
+      <c r="F387">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>13</v>
+      </c>
+      <c r="B388">
+        <v>1.2508E-3</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1</v>
+      </c>
+      <c r="D388">
+        <v>24</v>
+      </c>
+      <c r="E388" t="s">
+        <v>2</v>
+      </c>
+      <c r="F388">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>13</v>
+      </c>
+      <c r="B389">
+        <v>1.2351E-3</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1</v>
+      </c>
+      <c r="D389">
+        <v>24</v>
+      </c>
+      <c r="E389" t="s">
+        <v>2</v>
+      </c>
+      <c r="F389">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>13</v>
+      </c>
+      <c r="B390">
+        <v>1.2394999999999999E-3</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1</v>
+      </c>
+      <c r="D390">
+        <v>24</v>
+      </c>
+      <c r="E390" t="s">
+        <v>2</v>
+      </c>
+      <c r="F390">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>13</v>
+      </c>
+      <c r="B391">
+        <v>1.2681000000000001E-3</v>
+      </c>
+      <c r="C391" t="s">
+        <v>1</v>
+      </c>
+      <c r="D391">
+        <v>24</v>
+      </c>
+      <c r="E391" t="s">
+        <v>2</v>
+      </c>
+      <c r="F391">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>13</v>
+      </c>
+      <c r="B392">
+        <v>1.232E-3</v>
+      </c>
+      <c r="C392" t="s">
+        <v>1</v>
+      </c>
+      <c r="D392">
+        <v>24</v>
+      </c>
+      <c r="E392" t="s">
+        <v>2</v>
+      </c>
+      <c r="F392">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>13</v>
+      </c>
+      <c r="B393">
+        <v>1.2656E-3</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1</v>
+      </c>
+      <c r="D393">
+        <v>24</v>
+      </c>
+      <c r="E393" t="s">
+        <v>2</v>
+      </c>
+      <c r="F393">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>13</v>
+      </c>
+      <c r="B394">
+        <v>1.2712999999999999E-3</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1</v>
+      </c>
+      <c r="D394">
+        <v>24</v>
+      </c>
+      <c r="E394" t="s">
+        <v>2</v>
+      </c>
+      <c r="F394">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>13</v>
+      </c>
+      <c r="B395">
+        <v>1.2666999999999999E-3</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1</v>
+      </c>
+      <c r="D395">
+        <v>24</v>
+      </c>
+      <c r="E395" t="s">
+        <v>2</v>
+      </c>
+      <c r="F395">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>13</v>
+      </c>
+      <c r="B396">
+        <v>1.3086E-3</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1</v>
+      </c>
+      <c r="D396">
+        <v>24</v>
+      </c>
+      <c r="E396" t="s">
+        <v>2</v>
+      </c>
+      <c r="F396">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>13</v>
+      </c>
+      <c r="B397">
+        <v>1.2454E-3</v>
+      </c>
+      <c r="C397" t="s">
+        <v>1</v>
+      </c>
+      <c r="D397">
+        <v>24</v>
+      </c>
+      <c r="E397" t="s">
+        <v>2</v>
+      </c>
+      <c r="F397">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A398" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B398" s="15">
+        <f>SUM(B373:B397)/25</f>
+        <v>1.2688720000000001E-3</v>
+      </c>
+      <c r="C398" s="11"/>
+      <c r="D398" s="11"/>
+      <c r="E398" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F398" s="16">
+        <f>SUM(F373:F397)/25</f>
+        <v>23.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 2 plot files
</commit_message>
<xml_diff>
--- a/lab02/experiments/experiments.xlsx
+++ b/lab02/experiments/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\MHE\lab02\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD09F7-CB58-49CE-A0AA-59ED701B49DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1A0EB-3EE4-449C-BE63-5114AE281CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
                 <c:pt idx="2">
                   <c:v>1.2563119999999999E-3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="3" formatCode="0.0000000000">
                   <c:v>1.2688720000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -3522,7 +3522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O72" sqref="O72"/>
     </sheetView>
   </sheetViews>

</xml_diff>